<commit_message>
Remoção dos dados sensiveis no arquivo main
</commit_message>
<xml_diff>
--- a/Processados/nps_brasil_teste.xlsx
+++ b/Processados/nps_brasil_teste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaynan Ribeiro\Desktop\Git\Data_Quality_Homolog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaynan Ribeiro\Desktop\Git\Data_Quality\Processados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FB2F2F-5446-4F99-833F-DCB1D8BDA44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF5238B-79C9-4C35-AE46-AC201A3465A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dados" sheetId="1" r:id="rId1"/>
@@ -307,17 +307,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,14 +624,14 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
@@ -865,7 +864,7 @@
       <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9">
         <v>6</v>
       </c>
       <c r="F9" t="s">

</xml_diff>